<commit_message>
Added Queries to project
</commit_message>
<xml_diff>
--- a/GraphData/BCBS-Companies.xlsx
+++ b/GraphData/BCBS-Companies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Mitch Drive/MyProjects/BCBSA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitchd/Documents/MyProjects/BCBSA/GraphData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5D6964-AF55-904B-8F3E-A5FDE750E067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FFFCCF-8D57-BB49-9CB5-8255D597C523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9440" yWindow="7160" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{276D396F-EFBC-FF48-9446-433A3F0377BA}"/>
+    <workbookView xWindow="22120" yWindow="5600" windowWidth="20260" windowHeight="17440" activeTab="2" xr2:uid="{276D396F-EFBC-FF48-9446-433A3F0377BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="219">
   <si>
     <t>Alabama</t>
   </si>
@@ -673,6 +672,30 @@
   </si>
   <si>
     <t>Elevance Health</t>
+  </si>
+  <si>
+    <t>CAREFIRST</t>
+  </si>
+  <si>
+    <t>EXCELLUS</t>
+  </si>
+  <si>
+    <t>HARMARK</t>
+  </si>
+  <si>
+    <t>HIGHMARK</t>
+  </si>
+  <si>
+    <t>HORIZON</t>
+  </si>
+  <si>
+    <t>PREMERA</t>
+  </si>
+  <si>
+    <t>WELLMARK</t>
+  </si>
+  <si>
+    <t>ANTHEM</t>
   </si>
 </sst>
 </file>
@@ -2791,7 +2814,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>218</v>
       </c>
       <c r="B2" t="s">
         <v>210</v>
@@ -2975,7 +2998,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>111</v>
+        <v>211</v>
       </c>
       <c r="B25" t="s">
         <v>111</v>
@@ -2999,7 +3022,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>125</v>
+        <v>212</v>
       </c>
       <c r="B28" t="s">
         <v>125</v>
@@ -3007,7 +3030,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>194</v>
+        <v>213</v>
       </c>
       <c r="B29" t="s">
         <v>195</v>
@@ -3023,7 +3046,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>110</v>
+        <v>214</v>
       </c>
       <c r="B31" t="s">
         <v>110</v>
@@ -3031,7 +3054,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>126</v>
+        <v>215</v>
       </c>
       <c r="B32" t="s">
         <v>126</v>
@@ -3047,7 +3070,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>216</v>
       </c>
       <c r="B34" t="s">
         <v>115</v>
@@ -3063,7 +3086,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>114</v>
+        <v>217</v>
       </c>
       <c r="B36" t="s">
         <v>114</v>

</xml_diff>